<commit_message>
macro linear calculate for all store types
</commit_message>
<xml_diff>
--- a/Projects/TWEGAU/Data/Template.xlsx
+++ b/Projects/TWEGAU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Linear KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="64">
   <si>
     <t xml:space="preserve">kpi_parent_name</t>
   </si>
@@ -94,37 +94,37 @@
     <t xml:space="preserve">Fridge Door, Open Fridge, Ambient Shelf, Open Impulse Fridge, TWE Standalone Fridge, TWE Impulse Fridge Door, TWE Open Impulse Fridge, Impulse Fridge Door, Standalone Fridge</t>
   </si>
   <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelf_policy_from_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_of_shelves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">irrelevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_include_policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMON_ZONE1_SKU_ALL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Off Premise, Hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_OUT_OF_STORE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACRO_LINEAR_ALL_MANF_CAT_PER_SCENE_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shelf_policy_from_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number_of_shelves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">irrelevant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude_include_policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMON_ZONE1_SKU_ALL</t>
   </si>
   <si>
     <t xml:space="preserve">2,3</t>
@@ -650,20 +650,20 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.5663265306123"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="51.5663265306123"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="27.2704081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,9 +744,7 @@
       <c r="J2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="K2" s="6"/>
       <c r="L2" s="6" t="n">
         <v>0</v>
       </c>
@@ -760,10 +758,10 @@
         <v>18</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="121.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -771,10 +769,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>19</v>
@@ -789,9 +787,7 @@
       <c r="J3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="K3" s="6"/>
       <c r="L3" s="6" t="n">
         <v>0</v>
       </c>
@@ -805,19 +801,19 @@
         <v>19</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>19</v>
@@ -834,9 +830,7 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="K4" s="6"/>
       <c r="L4" s="9" t="n">
         <v>0</v>
       </c>
@@ -853,7 +847,7 @@
         <v>9</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -880,11 +874,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="45.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,7 +917,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>19</v>
@@ -940,7 +934,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>19</v>
@@ -973,7 +967,7 @@
   </sheetPr>
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
@@ -981,25 +975,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="49"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="48.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="44.2755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>3</v>
@@ -1034,10 +1028,10 @@
         <v>10</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>30</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
@@ -1046,10 +1040,10 @@
         <v>11</v>
       </c>
       <c r="O1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>32</v>
       </c>
       <c r="Q1" s="15" t="s">
         <v>14</v>
@@ -1063,10 +1057,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>1</v>
@@ -1078,7 +1072,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>34</v>
@@ -1100,7 +1094,7 @@
         <v>37</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>38</v>
@@ -1108,10 +1102,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="17" t="n">
         <v>1</v>
@@ -1123,7 +1117,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K3" s="17" t="s">
         <v>34</v>
@@ -1145,7 +1139,7 @@
         <v>37</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S3" s="17" t="s">
         <v>38</v>
@@ -1153,10 +1147,10 @@
     </row>
     <row r="4" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="17" t="n">
         <v>1</v>
@@ -1168,7 +1162,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>34</v>
@@ -1192,7 +1186,7 @@
         <v>37</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S4" s="17" t="s">
         <v>38</v>
@@ -1200,10 +1194,10 @@
     </row>
     <row r="5" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="17" t="n">
         <v>1</v>
@@ -1215,7 +1209,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K5" s="17" t="n">
         <v>2</v>
@@ -1237,7 +1231,7 @@
         <v>37</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S5" s="17" t="s">
         <v>38</v>
@@ -1245,10 +1239,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="17" t="n">
         <v>1</v>
@@ -1260,7 +1254,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>42</v>
@@ -1282,7 +1276,7 @@
         <v>37</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S6" s="17" t="s">
         <v>38</v>
@@ -1290,10 +1284,10 @@
     </row>
     <row r="7" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="17" t="n">
         <v>1</v>
@@ -1305,7 +1299,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K7" s="17" t="n">
         <v>2</v>
@@ -1329,7 +1323,7 @@
         <v>37</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S7" s="17" t="s">
         <v>38</v>
@@ -1337,10 +1331,10 @@
     </row>
     <row r="8" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="17" t="n">
         <v>1</v>
@@ -1352,7 +1346,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>42</v>
@@ -1376,7 +1370,7 @@
         <v>37</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S8" s="17" t="s">
         <v>38</v>
@@ -1399,7 +1393,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>34</v>
@@ -1423,7 +1417,7 @@
         <v>37</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S9" s="20" t="s">
         <v>38</v>
@@ -1446,7 +1440,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K10" s="20" t="n">
         <v>2</v>
@@ -1470,7 +1464,7 @@
         <v>37</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S10" s="20" t="s">
         <v>38</v>
@@ -1493,7 +1487,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K11" s="20" t="s">
         <v>42</v>
@@ -1517,7 +1511,7 @@
         <v>37</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S11" s="20" t="s">
         <v>38</v>
@@ -1540,7 +1534,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K12" s="23" t="n">
         <v>1</v>
@@ -1562,10 +1556,10 @@
         <v>37</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S12" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +1579,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K13" s="27" t="n">
         <v>4</v>
@@ -1607,10 +1601,10 @@
         <v>37</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S13" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1624,7 @@
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>51</v>
@@ -1652,10 +1646,10 @@
         <v>37</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S14" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,7 +1669,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K15" s="27" t="s">
         <v>51</v>
@@ -1697,10 +1691,10 @@
         <v>37</v>
       </c>
       <c r="R15" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S15" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1714,7 @@
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K16" s="27" t="n">
         <v>3</v>
@@ -1742,7 +1736,7 @@
         <v>37</v>
       </c>
       <c r="R16" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S16" s="27"/>
     </row>
@@ -1763,7 +1757,7 @@
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
       <c r="J17" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K17" s="27" t="s">
         <v>53</v>
@@ -1785,7 +1779,7 @@
         <v>37</v>
       </c>
       <c r="R17" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S17" s="27"/>
     </row>
@@ -1806,7 +1800,7 @@
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
       <c r="J18" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K18" s="27" t="s">
         <v>54</v>
@@ -1828,7 +1822,7 @@
         <v>37</v>
       </c>
       <c r="R18" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S18" s="27"/>
     </row>
@@ -1849,7 +1843,7 @@
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K19" s="27" t="s">
         <v>53</v>
@@ -1871,7 +1865,7 @@
         <v>37</v>
       </c>
       <c r="R19" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S19" s="27"/>
     </row>
@@ -1896,7 +1890,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>34</v>
@@ -1918,10 +1912,10 @@
         <v>18</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,7 +1939,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>34</v>
@@ -1967,10 +1961,10 @@
         <v>18</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,7 +1988,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>34</v>
@@ -2018,10 +2012,10 @@
         <v>18</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2039,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K23" s="17" t="n">
         <v>2</v>
@@ -2067,10 +2061,10 @@
         <v>18</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S23" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2094,7 +2088,7 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>42</v>
@@ -2116,10 +2110,10 @@
         <v>18</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S24" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,7 +2137,7 @@
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K25" s="17" t="n">
         <v>2</v>
@@ -2167,10 +2161,10 @@
         <v>18</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,7 +2188,7 @@
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K26" s="17" t="s">
         <v>42</v>
@@ -2218,10 +2212,10 @@
         <v>18</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,7 +2239,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K27" s="20" t="s">
         <v>34</v>
@@ -2269,10 +2263,10 @@
         <v>18</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S27" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,7 +2290,7 @@
       <c r="H28" s="21"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K28" s="20" t="s">
         <v>42</v>
@@ -2320,10 +2314,10 @@
         <v>18</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S28" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,7 +2341,7 @@
       <c r="H29" s="21"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K29" s="20" t="n">
         <v>2</v>
@@ -2371,10 +2365,10 @@
         <v>18</v>
       </c>
       <c r="R29" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S29" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,7 +2392,7 @@
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
       <c r="J30" s="23" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K30" s="23" t="n">
         <v>1</v>
@@ -2420,10 +2414,10 @@
         <v>18</v>
       </c>
       <c r="R30" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S30" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2447,7 +2441,7 @@
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K31" s="27" t="n">
         <v>4</v>
@@ -2469,10 +2463,10 @@
         <v>18</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S31" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +2490,7 @@
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K32" s="27" t="s">
         <v>51</v>
@@ -2518,10 +2512,10 @@
         <v>18</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S32" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2545,7 +2539,7 @@
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K33" s="27" t="s">
         <v>51</v>
@@ -2567,10 +2561,10 @@
         <v>18</v>
       </c>
       <c r="R33" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S33" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2588,7 @@
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
       <c r="J34" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K34" s="27" t="n">
         <v>3</v>
@@ -2616,10 +2610,10 @@
         <v>18</v>
       </c>
       <c r="R34" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S34" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,7 +2637,7 @@
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K35" s="27" t="s">
         <v>53</v>
@@ -2665,10 +2659,10 @@
         <v>18</v>
       </c>
       <c r="R35" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S35" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2692,7 +2686,7 @@
       <c r="H36" s="27"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K36" s="27" t="s">
         <v>53</v>
@@ -2714,10 +2708,10 @@
         <v>18</v>
       </c>
       <c r="R36" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S36" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,7 +2735,7 @@
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
       <c r="J37" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K37" s="27" t="s">
         <v>54</v>
@@ -2763,10 +2757,10 @@
         <v>18</v>
       </c>
       <c r="R37" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S37" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,7 +2788,7 @@
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K38" s="17" t="s">
         <v>34</v>
@@ -2817,7 +2811,7 @@
         <v>9</v>
       </c>
       <c r="S38" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,7 +2839,7 @@
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K39" s="17" t="s">
         <v>34</v>
@@ -2868,7 +2862,7 @@
         <v>9</v>
       </c>
       <c r="S39" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,7 +2890,7 @@
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K40" s="17" t="s">
         <v>34</v>
@@ -2921,7 +2915,7 @@
         <v>9</v>
       </c>
       <c r="S40" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,7 +2943,7 @@
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K41" s="17" t="n">
         <v>2</v>
@@ -2972,7 +2966,7 @@
         <v>9</v>
       </c>
       <c r="S41" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,7 +2994,7 @@
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K42" s="17" t="s">
         <v>42</v>
@@ -3021,7 +3015,7 @@
         <v>9</v>
       </c>
       <c r="S42" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,7 +3043,7 @@
       </c>
       <c r="I43" s="17"/>
       <c r="J43" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K43" s="17" t="n">
         <v>2</v>
@@ -3072,7 +3066,7 @@
         <v>9</v>
       </c>
       <c r="S43" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3100,7 +3094,7 @@
       </c>
       <c r="I44" s="17"/>
       <c r="J44" s="17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K44" s="17" t="s">
         <v>42</v>
@@ -3123,7 +3117,7 @@
         <v>9</v>
       </c>
       <c r="S44" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,7 +3145,7 @@
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K45" s="20" t="s">
         <v>34</v>
@@ -3176,7 +3170,7 @@
         <v>9</v>
       </c>
       <c r="S45" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,7 +3198,7 @@
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K46" s="20" t="s">
         <v>42</v>
@@ -3229,7 +3223,7 @@
         <v>9</v>
       </c>
       <c r="S46" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,7 +3251,7 @@
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K47" s="20" t="n">
         <v>2</v>
@@ -3282,7 +3276,7 @@
         <v>9</v>
       </c>
       <c r="S47" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3310,7 +3304,7 @@
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K48" s="23" t="n">
         <v>1</v>
@@ -3333,7 +3327,7 @@
         <v>9</v>
       </c>
       <c r="S48" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,7 +3355,7 @@
       </c>
       <c r="I49" s="27"/>
       <c r="J49" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K49" s="27" t="s">
         <v>54</v>
@@ -3384,7 +3378,7 @@
         <v>9</v>
       </c>
       <c r="S49" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,7 +3406,7 @@
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K50" s="27" t="s">
         <v>53</v>
@@ -3435,7 +3429,7 @@
         <v>9</v>
       </c>
       <c r="S50" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,7 +3457,7 @@
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K51" s="27" t="s">
         <v>53</v>
@@ -3486,7 +3480,7 @@
         <v>9</v>
       </c>
       <c r="S51" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3514,7 +3508,7 @@
       </c>
       <c r="I52" s="27"/>
       <c r="J52" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K52" s="27" t="n">
         <v>4</v>
@@ -3537,7 +3531,7 @@
         <v>9</v>
       </c>
       <c r="S52" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,7 +3559,7 @@
       </c>
       <c r="I53" s="27"/>
       <c r="J53" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K53" s="27" t="s">
         <v>51</v>
@@ -3588,7 +3582,7 @@
         <v>9</v>
       </c>
       <c r="S53" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3616,7 +3610,7 @@
       </c>
       <c r="I54" s="27"/>
       <c r="J54" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K54" s="27" t="s">
         <v>51</v>
@@ -3639,7 +3633,7 @@
         <v>9</v>
       </c>
       <c r="S54" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3667,7 +3661,7 @@
       </c>
       <c r="I55" s="27"/>
       <c r="J55" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K55" s="27" t="n">
         <v>3</v>
@@ -3690,7 +3684,7 @@
         <v>9</v>
       </c>
       <c r="S55" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3717,15 +3711,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="46.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix num-den-context for linear kpi
</commit_message>
<xml_diff>
--- a/Projects/TWEGAU/Data/Template.xlsx
+++ b/Projects/TWEGAU/Data/Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="65">
   <si>
     <t xml:space="preserve">kpi_parent_name</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">denominator_fk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">context_fk</t>
   </si>
   <si>
     <t xml:space="preserve">percentage</t>
@@ -648,25 +651,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="P24" activeCellId="0" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.5663265306123"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="51.5663265306123"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1023" min="11" style="2" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="2" width="26.0510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="21.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -718,31 +722,34 @@
       <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="113.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="n">
@@ -755,37 +762,40 @@
         <v>0</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="121.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="n">
@@ -798,35 +808,38 @@
         <v>0</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -841,13 +854,16 @@
         <v>0</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>24</v>
+      <c r="Q4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -868,17 +884,17 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,53 +916,53 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -967,33 +983,33 @@
   </sheetPr>
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
+      <selection pane="bottomLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="48.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="42.6581632653061"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="14" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="14" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>3</v>
@@ -1028,10 +1044,10 @@
         <v>10</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
@@ -1040,10 +1056,10 @@
         <v>11</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q1" s="15" t="s">
         <v>14</v>
@@ -1052,15 +1068,15 @@
         <v>15</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>1</v>
@@ -1072,40 +1088,40 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L2" s="17" t="n">
         <v>4</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N2" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P2" s="17"/>
       <c r="Q2" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="17" t="n">
         <v>1</v>
@@ -1117,40 +1133,40 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L3" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P3" s="17"/>
       <c r="Q3" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="17" t="n">
         <v>1</v>
@@ -1162,42 +1178,42 @@
       <c r="H4" s="18"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L4" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="N4" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="17" t="n">
         <v>1</v>
@@ -1209,7 +1225,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K5" s="17" t="n">
         <v>2</v>
@@ -1218,31 +1234,31 @@
         <v>3</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N5" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P5" s="17"/>
       <c r="Q5" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="17" t="n">
         <v>1</v>
@@ -1254,40 +1270,40 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N6" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P6" s="17"/>
       <c r="Q6" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S6" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="17" t="n">
         <v>1</v>
@@ -1299,7 +1315,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K7" s="17" t="n">
         <v>2</v>
@@ -1308,33 +1324,33 @@
         <v>4</v>
       </c>
       <c r="M7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="N7" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="17" t="n">
         <v>1</v>
@@ -1346,42 +1362,42 @@
       <c r="H8" s="18"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="N8" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="20" t="n">
         <v>2</v>
@@ -1393,42 +1409,42 @@
       <c r="H9" s="21"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L9" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="N9" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="20" t="n">
         <v>2</v>
@@ -1440,7 +1456,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K10" s="20" t="n">
         <v>2</v>
@@ -1449,33 +1465,33 @@
         <v>4</v>
       </c>
       <c r="M10" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="N10" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="20" t="n">
         <v>2</v>
@@ -1487,42 +1503,42 @@
       <c r="H11" s="21"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M11" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S11" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="N11" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P11" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="23" t="n">
         <v>3</v>
@@ -1534,40 +1550,40 @@
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K12" s="23" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N12" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P12" s="23"/>
       <c r="Q12" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S12" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="27" t="n">
         <v>4</v>
@@ -1579,7 +1595,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K13" s="27" t="n">
         <v>4</v>
@@ -1588,31 +1604,31 @@
         <v>4</v>
       </c>
       <c r="M13" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N13" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P13" s="27"/>
       <c r="Q13" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S13" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="27" t="n">
         <v>4</v>
@@ -1624,40 +1640,40 @@
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L14" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N14" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O14" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P14" s="27"/>
       <c r="Q14" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S14" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="27" t="n">
         <v>4</v>
@@ -1669,40 +1685,40 @@
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L15" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M15" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N15" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P15" s="27"/>
       <c r="Q15" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R15" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S15" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="27" t="n">
         <v>4</v>
@@ -1714,7 +1730,7 @@
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K16" s="27" t="n">
         <v>3</v>
@@ -1723,29 +1739,29 @@
         <v>3</v>
       </c>
       <c r="M16" s="28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N16" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P16" s="27"/>
       <c r="Q16" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R16" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="27" t="n">
         <v>4</v>
@@ -1757,38 +1773,38 @@
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
       <c r="J17" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K17" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L17" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N17" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O17" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P17" s="27"/>
       <c r="Q17" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R17" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="27" t="n">
         <v>4</v>
@@ -1800,38 +1816,38 @@
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
       <c r="J18" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K18" s="27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L18" s="27" t="n">
         <v>4</v>
       </c>
       <c r="M18" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N18" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O18" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P18" s="27"/>
       <c r="Q18" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R18" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S18" s="27"/>
     </row>
     <row r="19" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" s="27" t="n">
         <v>4</v>
@@ -1843,203 +1859,203 @@
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K19" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L19" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N19" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P19" s="27"/>
       <c r="Q19" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R19" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S19" s="27"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L20" s="17" t="n">
         <v>4</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P20" s="17"/>
       <c r="Q20" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L21" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N21" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P21" s="17"/>
       <c r="Q21" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L22" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N22" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S22" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="47.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K23" s="17" t="n">
         <v>2</v>
@@ -2048,96 +2064,96 @@
         <v>3</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N23" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P23" s="17"/>
       <c r="Q23" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S23" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N24" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P24" s="17"/>
       <c r="Q24" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S24" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K25" s="17" t="n">
         <v>2</v>
@@ -2146,202 +2162,202 @@
         <v>4</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N25" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q25" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N26" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P26" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q26" s="30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L27" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N27" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q27" s="32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S27" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L28" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N28" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P28" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q28" s="32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S28" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="21"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K29" s="20" t="n">
         <v>2</v>
@@ -2350,98 +2366,98 @@
         <v>4</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N29" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q29" s="32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R29" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S29" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="116.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C30" s="23" t="n">
         <v>3</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
       <c r="J30" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K30" s="23" t="n">
         <v>1</v>
       </c>
       <c r="L30" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M30" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N30" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O30" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P30" s="23"/>
       <c r="Q30" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R30" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S30" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K31" s="27" t="n">
         <v>4</v>
@@ -2450,145 +2466,145 @@
         <v>4</v>
       </c>
       <c r="M31" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N31" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O31" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P31" s="27"/>
       <c r="Q31" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S31" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C32" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K32" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L32" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M32" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N32" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O32" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P32" s="27"/>
       <c r="Q32" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S32" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K33" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L33" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N33" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O33" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P33" s="27"/>
       <c r="Q33" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R33" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S33" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C34" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
       <c r="J34" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K34" s="27" t="n">
         <v>3</v>
@@ -2597,201 +2613,201 @@
         <v>3</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N34" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O34" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P34" s="27"/>
       <c r="Q34" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R34" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S34" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K35" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L35" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M35" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N35" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O35" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P35" s="27"/>
       <c r="Q35" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R35" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S35" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C36" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H36" s="27"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K36" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L36" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M36" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N36" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O36" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P36" s="27"/>
       <c r="Q36" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R36" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S36" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="59.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C37" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
       <c r="J37" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K37" s="27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L37" s="27" t="n">
         <v>4</v>
       </c>
       <c r="M37" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N37" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O37" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P37" s="27"/>
       <c r="Q37" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R37" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S37" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C38" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L38" s="17" t="n">
         <v>4</v>
@@ -2801,48 +2817,48 @@
         <v>1</v>
       </c>
       <c r="O38" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P38" s="17"/>
       <c r="Q38" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R38" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S38" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C39" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L39" s="17" t="n">
         <v>5</v>
@@ -2852,48 +2868,48 @@
         <v>1</v>
       </c>
       <c r="O39" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P39" s="17"/>
       <c r="Q39" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R39" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S39" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L40" s="17" t="n">
         <v>5</v>
@@ -2903,47 +2919,47 @@
         <v>1</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P40" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q40" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R40" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S40" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E41" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K41" s="17" t="n">
         <v>2</v>
@@ -2956,51 +2972,51 @@
         <v>1</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P41" s="17"/>
       <c r="Q41" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R41" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S41" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E42" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M42" s="17"/>
       <c r="N42" s="17" t="n">
@@ -3009,41 +3025,41 @@
       <c r="O42" s="17"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R42" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S42" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C43" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I43" s="17"/>
       <c r="J43" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K43" s="17" t="n">
         <v>2</v>
@@ -3057,50 +3073,50 @@
       </c>
       <c r="O43" s="17"/>
       <c r="P43" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q43" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R43" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S43" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C44" s="17" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I44" s="17"/>
       <c r="J44" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17" t="n">
@@ -3108,47 +3124,47 @@
       </c>
       <c r="O44" s="17"/>
       <c r="P44" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q44" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R44" s="17" t="s">
         <v>9</v>
       </c>
       <c r="S44" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C45" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>9</v>
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L45" s="20" t="n">
         <v>5</v>
@@ -3158,100 +3174,100 @@
         <v>1</v>
       </c>
       <c r="O45" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q45" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R45" s="20" t="s">
         <v>9</v>
       </c>
       <c r="S45" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C46" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L46" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M46" s="21"/>
       <c r="N46" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O46" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P46" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q46" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R46" s="20" t="s">
         <v>9</v>
       </c>
       <c r="S46" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C47" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K47" s="20" t="n">
         <v>2</v>
@@ -3264,101 +3280,101 @@
         <v>1</v>
       </c>
       <c r="O47" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P47" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q47" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R47" s="20" t="s">
         <v>9</v>
       </c>
       <c r="S47" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C48" s="23" t="n">
         <v>3</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="23"/>
       <c r="G48" s="24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K48" s="23" t="n">
         <v>1</v>
       </c>
       <c r="L48" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M48" s="23"/>
       <c r="N48" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O48" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P48" s="23"/>
       <c r="Q48" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R48" s="23" t="s">
         <v>9</v>
       </c>
       <c r="S48" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C49" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E49" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H49" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I49" s="27"/>
       <c r="J49" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K49" s="27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L49" s="27" t="n">
         <v>4</v>
@@ -3368,147 +3384,147 @@
         <v>1</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P49" s="27"/>
       <c r="Q49" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R49" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S49" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C50" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E50" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L50" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M50" s="27"/>
       <c r="N50" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O50" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P50" s="27"/>
       <c r="Q50" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R50" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S50" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C51" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F51" s="27"/>
       <c r="G51" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K51" s="27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L51" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M51" s="27"/>
       <c r="N51" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O51" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P51" s="27"/>
       <c r="Q51" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R51" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S51" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C52" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E52" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I52" s="27"/>
       <c r="J52" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K52" s="27" t="n">
         <v>4</v>
@@ -3521,48 +3537,48 @@
         <v>1</v>
       </c>
       <c r="O52" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P52" s="27"/>
       <c r="Q52" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R52" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S52" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C53" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E53" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I53" s="27"/>
       <c r="J53" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K53" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L53" s="27" t="n">
         <v>5</v>
@@ -3572,48 +3588,48 @@
         <v>1</v>
       </c>
       <c r="O53" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P53" s="27"/>
       <c r="Q53" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R53" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S53" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C54" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E54" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I54" s="27"/>
       <c r="J54" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K54" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L54" s="27" t="n">
         <v>5</v>
@@ -3623,45 +3639,45 @@
         <v>1</v>
       </c>
       <c r="O54" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P54" s="27"/>
       <c r="Q54" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R54" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S54" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C55" s="27" t="n">
         <v>4</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E55" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H55" s="28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I55" s="27"/>
       <c r="J55" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K55" s="27" t="n">
         <v>3</v>
@@ -3674,17 +3690,17 @@
         <v>1</v>
       </c>
       <c r="O55" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P55" s="27"/>
       <c r="Q55" s="27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R55" s="27" t="s">
         <v>9</v>
       </c>
       <c r="S55" s="27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3705,21 +3721,21 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3744,14 +3760,14 @@
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="9"/>
       <c r="G2" s="34"/>
@@ -3760,14 +3776,14 @@
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="9"/>
       <c r="G3" s="34"/>
@@ -3776,14 +3792,14 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9"/>
       <c r="G4" s="34"/>
@@ -3792,14 +3808,14 @@
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="9"/>
       <c r="G5" s="34"/>
@@ -3808,54 +3824,54 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5"/>
       <c r="G6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5"/>
     </row>

</xml_diff>

<commit_message>
make own and all same
</commit_message>
<xml_diff>
--- a/Projects/TWEGAU/Data/Template.xlsx
+++ b/Projects/TWEGAU/Data/Template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="64">
   <si>
     <t xml:space="preserve">kpi_parent_name</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White Wine</t>
   </si>
   <si>
     <t xml:space="preserve">Fridge Door, Open Fridge, Ambient Shelf, Open Impulse Fridge, TWE Standalone Fridge, TWE Impulse Fridge Door, TWE Open Impulse Fridge, Impulse Fridge Door, Standalone Fridge</t>
@@ -654,20 +651,20 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topRight" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="2" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="2" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="40.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="2" width="24.5663265306122"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="21.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -726,7 +723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="56.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>18</v>
@@ -745,11 +742,11 @@
         <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="n">
@@ -765,13 +762,13 @@
         <v>20</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,10 +776,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>19</v>
@@ -799,7 +796,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="n">
@@ -815,22 +812,22 @@
         <v>20</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="80.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>9</v>
@@ -842,7 +839,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>21</v>
@@ -871,7 +868,7 @@
         <v>19</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -898,11 +895,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="50.4795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="49.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,7 +938,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>20</v>
@@ -958,7 +955,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>20</v>
@@ -999,23 +996,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="14" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="14" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="14" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="14" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="14" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="14" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="14" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="14" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="14" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>3</v>
@@ -1050,10 +1047,10 @@
         <v>10</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>30</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
@@ -1062,10 +1059,10 @@
         <v>11</v>
       </c>
       <c r="O1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>32</v>
       </c>
       <c r="Q1" s="15" t="s">
         <v>14</v>
@@ -1079,10 +1076,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>1</v>
@@ -1095,37 +1092,37 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>35</v>
-      </c>
       <c r="N2" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P2" s="17"/>
       <c r="Q2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="17" t="n">
         <v>1</v>
@@ -1138,37 +1135,37 @@
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
       <c r="K3" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N3" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P3" s="17"/>
       <c r="Q3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="17" t="n">
         <v>1</v>
@@ -1181,39 +1178,39 @@
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L4" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="17" t="s">
+      <c r="Q4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="17" t="s">
+      <c r="R4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="17" t="n">
         <v>1</v>
@@ -1232,31 +1229,31 @@
         <v>3</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P5" s="17"/>
       <c r="Q5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="17" t="n">
         <v>1</v>
@@ -1269,37 +1266,37 @@
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="M6" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N6" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P6" s="17"/>
       <c r="Q6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="17" t="n">
         <v>1</v>
@@ -1318,33 +1315,33 @@
         <v>4</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N7" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="17" t="s">
+      <c r="R7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="17" t="n">
         <v>1</v>
@@ -1357,39 +1354,39 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="M8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="17" t="s">
+      <c r="Q8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" s="17" t="s">
+      <c r="R8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S8" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="20" t="n">
         <v>2</v>
@@ -1402,39 +1399,39 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L9" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N9" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="20" t="s">
+      <c r="R9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="R9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S9" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="20" t="n">
         <v>2</v>
@@ -1453,33 +1450,33 @@
         <v>4</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N10" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O10" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q10" s="20" t="s">
+      <c r="R10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="20" t="n">
         <v>2</v>
@@ -1492,39 +1489,39 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="M11" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N11" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O11" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" s="20" t="s">
+      <c r="R11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S11" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="23" t="n">
         <v>3</v>
@@ -1540,34 +1537,34 @@
         <v>1</v>
       </c>
       <c r="L12" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="25" t="s">
-        <v>49</v>
-      </c>
       <c r="N12" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P12" s="23"/>
       <c r="Q12" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S12" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="27" t="n">
         <v>4</v>
@@ -1586,31 +1583,31 @@
         <v>4</v>
       </c>
       <c r="M13" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P13" s="27"/>
       <c r="Q13" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S13" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="27" t="n">
         <v>4</v>
@@ -1623,37 +1620,37 @@
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L14" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O14" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P14" s="27"/>
       <c r="Q14" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S14" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="27" t="n">
         <v>4</v>
@@ -1666,37 +1663,37 @@
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L15" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M15" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N15" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P15" s="27"/>
       <c r="Q15" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R15" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S15" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="27" t="n">
         <v>4</v>
@@ -1715,29 +1712,29 @@
         <v>3</v>
       </c>
       <c r="M16" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N16" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P16" s="27"/>
       <c r="Q16" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R16" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="27" t="n">
         <v>4</v>
@@ -1750,35 +1747,35 @@
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
       <c r="K17" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L17" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O17" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P17" s="27"/>
       <c r="Q17" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R17" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="27" t="n">
         <v>4</v>
@@ -1791,35 +1788,35 @@
       <c r="I18" s="27"/>
       <c r="J18" s="27"/>
       <c r="K18" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L18" s="27" t="n">
         <v>4</v>
       </c>
       <c r="M18" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N18" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O18" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P18" s="27"/>
       <c r="Q18" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R18" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S18" s="27"/>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="27" t="n">
         <v>4</v>
@@ -1832,35 +1829,35 @@
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
       <c r="K19" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N19" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P19" s="27"/>
       <c r="Q19" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R19" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S19" s="27"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="17" t="n">
         <v>1</v>
@@ -1871,43 +1868,43 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
       <c r="K20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>35</v>
-      </c>
       <c r="N20" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P20" s="17"/>
       <c r="Q20" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="17" t="n">
         <v>1</v>
@@ -1918,43 +1915,43 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
       <c r="K21" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L21" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N21" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P21" s="17"/>
       <c r="Q21" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>1</v>
@@ -1965,45 +1962,45 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L22" s="17" t="n">
         <v>5</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N22" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P22" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q22" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S22" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="17" t="n">
         <v>1</v>
@@ -2014,7 +2011,7 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -2026,31 +2023,31 @@
         <v>3</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N23" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P23" s="17"/>
       <c r="Q23" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S23" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="17" t="n">
         <v>1</v>
@@ -2061,43 +2058,43 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="M24" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N24" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P24" s="17"/>
       <c r="Q24" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S24" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="17" t="n">
         <v>1</v>
@@ -2108,7 +2105,7 @@
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
@@ -2120,33 +2117,33 @@
         <v>4</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N25" s="17" t="n">
         <v>1</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q25" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="17" t="n">
         <v>1</v>
@@ -2157,45 +2154,45 @@
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L26" s="17" t="s">
+      <c r="M26" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N26" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P26" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="M26" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="O26" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" s="17" t="s">
-        <v>44</v>
-      </c>
       <c r="Q26" s="30" t="s">
         <v>19</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="20" t="n">
         <v>2</v>
@@ -2206,45 +2203,45 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
       <c r="K27" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L27" s="20" t="n">
         <v>5</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N27" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P27" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q27" s="32" t="s">
         <v>19</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S27" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="20" t="n">
         <v>2</v>
@@ -2255,45 +2252,45 @@
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
       <c r="K28" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="L28" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="M28" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N28" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P28" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q28" s="32" t="s">
         <v>19</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S28" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="20" t="n">
         <v>2</v>
@@ -2304,7 +2301,7 @@
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" s="21"/>
       <c r="I29" s="20"/>
@@ -2316,33 +2313,33 @@
         <v>4</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N29" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q29" s="32" t="s">
         <v>19</v>
       </c>
       <c r="R29" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S29" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="23" t="n">
         <v>3</v>
@@ -2353,7 +2350,7 @@
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
@@ -2362,34 +2359,34 @@
         <v>1</v>
       </c>
       <c r="L30" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="M30" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="M30" s="25" t="s">
-        <v>49</v>
-      </c>
       <c r="N30" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O30" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P30" s="23"/>
       <c r="Q30" s="23" t="s">
         <v>19</v>
       </c>
       <c r="R30" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S30" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="27" t="n">
         <v>4</v>
@@ -2400,7 +2397,7 @@
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
@@ -2412,31 +2409,31 @@
         <v>4</v>
       </c>
       <c r="M31" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N31" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O31" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P31" s="27"/>
       <c r="Q31" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R31" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S31" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="27" t="n">
         <v>4</v>
@@ -2447,43 +2444,43 @@
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
       <c r="K32" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L32" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M32" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N32" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O32" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P32" s="27"/>
       <c r="Q32" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R32" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S32" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="27" t="n">
         <v>4</v>
@@ -2494,43 +2491,43 @@
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
       <c r="K33" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L33" s="27" t="n">
         <v>5</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N33" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O33" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P33" s="27"/>
       <c r="Q33" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R33" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S33" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="27" t="n">
         <v>4</v>
@@ -2541,7 +2538,7 @@
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
@@ -2553,31 +2550,31 @@
         <v>3</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N34" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O34" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P34" s="27"/>
       <c r="Q34" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R34" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S34" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="27" t="n">
         <v>4</v>
@@ -2588,43 +2585,43 @@
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
       <c r="K35" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L35" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M35" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N35" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O35" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P35" s="27"/>
       <c r="Q35" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R35" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S35" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="27" t="n">
         <v>4</v>
@@ -2635,43 +2632,43 @@
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H36" s="27"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
       <c r="K36" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L36" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M36" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N36" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O36" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P36" s="27"/>
       <c r="Q36" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R36" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S36" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="27" t="n">
         <v>4</v>
@@ -2682,43 +2679,43 @@
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
       <c r="K37" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L37" s="27" t="n">
         <v>4</v>
       </c>
       <c r="M37" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N37" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O37" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P37" s="27"/>
       <c r="Q37" s="27" t="s">
         <v>19</v>
       </c>
       <c r="R37" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S37" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="17" t="n">
         <v>1</v>
@@ -2731,15 +2728,15 @@
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L38" s="17" t="n">
         <v>4</v>
@@ -2749,7 +2746,7 @@
         <v>1</v>
       </c>
       <c r="O38" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P38" s="17"/>
       <c r="Q38" s="17" t="s">
@@ -2759,15 +2756,15 @@
         <v>9</v>
       </c>
       <c r="S38" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="17" t="n">
         <v>1</v>
@@ -2780,15 +2777,15 @@
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L39" s="17" t="n">
         <v>5</v>
@@ -2798,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="O39" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P39" s="17"/>
       <c r="Q39" s="17" t="s">
@@ -2808,15 +2805,15 @@
         <v>9</v>
       </c>
       <c r="S39" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>1</v>
@@ -2829,15 +2826,15 @@
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L40" s="17" t="n">
         <v>5</v>
@@ -2847,10 +2844,10 @@
         <v>1</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P40" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q40" s="17" t="s">
         <v>19</v>
@@ -2859,15 +2856,15 @@
         <v>9</v>
       </c>
       <c r="S40" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="17" t="n">
         <v>1</v>
@@ -2880,10 +2877,10 @@
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
@@ -2898,7 +2895,7 @@
         <v>1</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P41" s="17"/>
       <c r="Q41" s="17" t="s">
@@ -2908,15 +2905,15 @@
         <v>9</v>
       </c>
       <c r="S41" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="17" t="n">
         <v>1</v>
@@ -2929,18 +2926,18 @@
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L42" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="M42" s="17"/>
       <c r="N42" s="17" t="n">
@@ -2955,15 +2952,15 @@
         <v>9</v>
       </c>
       <c r="S42" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="17" t="n">
         <v>1</v>
@@ -2976,10 +2973,10 @@
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
@@ -2995,7 +2992,7 @@
       </c>
       <c r="O43" s="17"/>
       <c r="P43" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q43" s="17" t="s">
         <v>19</v>
@@ -3004,15 +3001,15 @@
         <v>9</v>
       </c>
       <c r="S43" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="17" t="n">
         <v>1</v>
@@ -3025,18 +3022,18 @@
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
       <c r="K44" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L44" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17" t="n">
@@ -3044,7 +3041,7 @@
       </c>
       <c r="O44" s="17"/>
       <c r="P44" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q44" s="17" t="s">
         <v>19</v>
@@ -3053,15 +3050,15 @@
         <v>9</v>
       </c>
       <c r="S44" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" s="20" t="n">
         <v>2</v>
@@ -3074,15 +3071,15 @@
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L45" s="20" t="n">
         <v>5</v>
@@ -3092,10 +3089,10 @@
         <v>1</v>
       </c>
       <c r="O45" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q45" s="20" t="s">
         <v>19</v>
@@ -3104,15 +3101,15 @@
         <v>9</v>
       </c>
       <c r="S45" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="20" t="n">
         <v>2</v>
@@ -3125,28 +3122,28 @@
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
       <c r="K46" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L46" s="20" t="s">
         <v>42</v>
-      </c>
-      <c r="L46" s="20" t="s">
-        <v>43</v>
       </c>
       <c r="M46" s="21"/>
       <c r="N46" s="20" t="n">
         <v>1</v>
       </c>
       <c r="O46" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P46" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q46" s="20" t="s">
         <v>19</v>
@@ -3155,15 +3152,15 @@
         <v>9</v>
       </c>
       <c r="S46" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="20" t="n">
         <v>2</v>
@@ -3176,10 +3173,10 @@
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -3194,10 +3191,10 @@
         <v>1</v>
       </c>
       <c r="O47" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P47" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q47" s="20" t="s">
         <v>19</v>
@@ -3206,15 +3203,15 @@
         <v>9</v>
       </c>
       <c r="S47" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="23" t="n">
         <v>3</v>
@@ -3227,10 +3224,10 @@
       </c>
       <c r="F48" s="23"/>
       <c r="G48" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23"/>
@@ -3238,14 +3235,14 @@
         <v>1</v>
       </c>
       <c r="L48" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M48" s="23"/>
       <c r="N48" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O48" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P48" s="23"/>
       <c r="Q48" s="23" t="s">
@@ -3255,15 +3252,15 @@
         <v>9</v>
       </c>
       <c r="S48" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="27" t="n">
         <v>4</v>
@@ -3276,15 +3273,15 @@
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H49" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
       <c r="K49" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L49" s="27" t="n">
         <v>4</v>
@@ -3294,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="O49" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P49" s="27"/>
       <c r="Q49" s="27" t="s">
@@ -3304,15 +3301,15 @@
         <v>9</v>
       </c>
       <c r="S49" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="27" t="n">
         <v>4</v>
@@ -3325,25 +3322,25 @@
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27"/>
       <c r="K50" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L50" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M50" s="27"/>
       <c r="N50" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O50" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P50" s="27"/>
       <c r="Q50" s="27" t="s">
@@ -3353,15 +3350,15 @@
         <v>9</v>
       </c>
       <c r="S50" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="27" t="n">
         <v>4</v>
@@ -3374,25 +3371,25 @@
       </c>
       <c r="F51" s="27"/>
       <c r="G51" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
       <c r="K51" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L51" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M51" s="27"/>
       <c r="N51" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O51" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P51" s="27"/>
       <c r="Q51" s="27" t="s">
@@ -3402,15 +3399,15 @@
         <v>9</v>
       </c>
       <c r="S51" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="27" t="n">
         <v>4</v>
@@ -3423,10 +3420,10 @@
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
@@ -3441,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="O52" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P52" s="27"/>
       <c r="Q52" s="27" t="s">
@@ -3451,15 +3448,15 @@
         <v>9</v>
       </c>
       <c r="S52" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" s="27" t="n">
         <v>4</v>
@@ -3472,15 +3469,15 @@
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I53" s="27"/>
       <c r="J53" s="27"/>
       <c r="K53" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L53" s="27" t="n">
         <v>5</v>
@@ -3490,7 +3487,7 @@
         <v>1</v>
       </c>
       <c r="O53" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P53" s="27"/>
       <c r="Q53" s="27" t="s">
@@ -3500,15 +3497,15 @@
         <v>9</v>
       </c>
       <c r="S53" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="27" t="n">
         <v>4</v>
@@ -3521,15 +3518,15 @@
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
       <c r="K54" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L54" s="27" t="n">
         <v>5</v>
@@ -3539,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="O54" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P54" s="27"/>
       <c r="Q54" s="27" t="s">
@@ -3549,15 +3546,15 @@
         <v>9</v>
       </c>
       <c r="S54" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="27" t="n">
         <v>4</v>
@@ -3570,10 +3567,10 @@
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H55" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
@@ -3588,7 +3585,7 @@
         <v>1</v>
       </c>
       <c r="O55" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P55" s="27"/>
       <c r="Q55" s="27" t="s">
@@ -3598,7 +3595,7 @@
         <v>9</v>
       </c>
       <c r="S55" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3625,14 +3622,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="33" width="7.1530612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -3658,14 +3655,14 @@
     </row>
     <row r="2" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="9"/>
       <c r="G2" s="34"/>
@@ -3674,14 +3671,14 @@
     </row>
     <row r="3" customFormat="false" ht="31.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="9"/>
       <c r="G3" s="34"/>
@@ -3690,14 +3687,14 @@
     </row>
     <row r="4" customFormat="false" ht="38.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="9"/>
       <c r="G4" s="34"/>
@@ -3706,14 +3703,14 @@
     </row>
     <row r="5" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="9"/>
       <c r="G5" s="34"/>
@@ -3722,54 +3719,54 @@
     </row>
     <row r="6" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5"/>
       <c r="G6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="29.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="5"/>
     </row>

</xml_diff>